<commit_message>
Swapped Brython and PyPy.js
</commit_message>
<xml_diff>
--- a/benchmarks/Benchmarks.xlsx
+++ b/benchmarks/Benchmarks.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pa-pyscript\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE9AD31-5925-42DC-9F1E-29B06AD0C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FCC154-C190-4926-B74F-8C9C77788DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="-13215" windowWidth="21600" windowHeight="11385" xr2:uid="{62393A8A-AA59-423C-856C-210751BB75C5}"/>
+    <workbookView xWindow="2925" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{62393A8A-AA59-423C-856C-210751BB75C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="CPython" sheetId="1" r:id="rId2"/>
     <sheet name="Skulpt" sheetId="4" r:id="rId3"/>
-    <sheet name="PyPy.js" sheetId="3" r:id="rId4"/>
-    <sheet name="Brython" sheetId="5" r:id="rId5"/>
+    <sheet name="Brython" sheetId="5" r:id="rId4"/>
+    <sheet name="PyPy.js" sheetId="3" r:id="rId5"/>
     <sheet name="Pyodide" sheetId="6" r:id="rId6"/>
     <sheet name="PyScript" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="24">
   <si>
     <t>assignment.py</t>
   </si>
@@ -112,11 +112,17 @@
   <si>
     <t>x-mal langsamer als CPython</t>
   </si>
+  <si>
+    <t>Durchschnitt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -147,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -272,11 +278,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,29 +360,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -639,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0390DB9F-7ACF-4DCE-B0A0-C83D8503FC6D}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -651,28 +719,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="21"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
@@ -680,10 +748,10 @@
         <v>17</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>19</v>
@@ -691,17 +759,17 @@
       <c r="G2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>19</v>
@@ -711,7 +779,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8">
@@ -721,10 +789,10 @@
         <v>1711</v>
       </c>
       <c r="D3" s="8">
+        <v>1242</v>
+      </c>
+      <c r="E3" s="8">
         <v>1602</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1242</v>
       </c>
       <c r="F3" s="8">
         <v>221</v>
@@ -732,33 +800,33 @@
       <c r="G3" s="9">
         <v>194</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="15">
         <f>ROUND(B3/$B3,2)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="8">
-        <f>ROUND(C3/$B3,1)</f>
+      <c r="I3" s="30">
+        <f t="shared" ref="I3:I14" si="0">ROUND(C3/$B3,2)</f>
         <v>36.4</v>
       </c>
-      <c r="J3" s="8">
-        <f t="shared" ref="J3:J14" si="0">ROUND(D3/$B3,1)</f>
-        <v>34.1</v>
-      </c>
-      <c r="K3" s="8">
-        <f t="shared" ref="K3:K14" si="1">ROUND(E3/$B3,1)</f>
-        <v>26.4</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" ref="L3:L14" si="2">ROUND(F3/$B3,1)</f>
+      <c r="J3" s="30">
+        <f t="shared" ref="J3:J14" si="1">ROUND(D3/$B3,2)</f>
+        <v>26.43</v>
+      </c>
+      <c r="K3" s="30">
+        <f t="shared" ref="K3:K14" si="2">ROUND(E3/$B3,2)</f>
+        <v>34.090000000000003</v>
+      </c>
+      <c r="L3" s="30">
+        <f t="shared" ref="L3:L14" si="3">ROUND(F3/$B3,2)</f>
         <v>4.7</v>
       </c>
-      <c r="M3" s="9">
-        <f t="shared" ref="M3:M14" si="3">ROUND(G3/$B3,1)</f>
-        <v>4.0999999999999996</v>
+      <c r="M3" s="31">
+        <f t="shared" ref="M3:M14" si="4">ROUND(G3/$B3,2)</f>
+        <v>4.13</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="8">
@@ -768,10 +836,10 @@
         <v>2919</v>
       </c>
       <c r="D4" s="8">
+        <v>2116</v>
+      </c>
+      <c r="E4" s="8">
         <v>1828</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2116</v>
       </c>
       <c r="F4" s="8">
         <v>378</v>
@@ -779,33 +847,33 @@
       <c r="G4" s="9">
         <v>325</v>
       </c>
-      <c r="H4" s="18">
-        <f t="shared" ref="H4:H14" si="4">ROUND(B4/$B4,2)</f>
+      <c r="H4" s="15">
+        <f t="shared" ref="H4:H14" si="5">ROUND(B4/$B4,2)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="8">
-        <f t="shared" ref="I4:I14" si="5">ROUND(C4/$B4,1)</f>
-        <v>30.1</v>
-      </c>
-      <c r="J4" s="8">
-        <f t="shared" si="0"/>
-        <v>18.8</v>
-      </c>
-      <c r="K4" s="8">
-        <f t="shared" si="1"/>
-        <v>21.8</v>
-      </c>
-      <c r="L4" s="8">
+      <c r="I4" s="30">
+        <f t="shared" si="0"/>
+        <v>30.09</v>
+      </c>
+      <c r="J4" s="30">
+        <f t="shared" si="1"/>
+        <v>21.81</v>
+      </c>
+      <c r="K4" s="30">
         <f t="shared" si="2"/>
+        <v>18.850000000000001</v>
+      </c>
+      <c r="L4" s="30">
+        <f t="shared" si="3"/>
         <v>3.9</v>
       </c>
-      <c r="M4" s="9">
-        <f t="shared" si="3"/>
-        <v>3.4</v>
+      <c r="M4" s="31">
+        <f t="shared" si="4"/>
+        <v>3.35</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="8">
@@ -815,10 +883,10 @@
         <v>1707</v>
       </c>
       <c r="D5" s="8">
+        <v>1306</v>
+      </c>
+      <c r="E5" s="8">
         <v>1505</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1306</v>
       </c>
       <c r="F5" s="8">
         <v>234</v>
@@ -826,33 +894,33 @@
       <c r="G5" s="9">
         <v>195</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" si="0"/>
+        <v>38.799999999999997</v>
+      </c>
+      <c r="J5" s="30">
+        <f t="shared" si="1"/>
+        <v>29.68</v>
+      </c>
+      <c r="K5" s="30">
+        <f t="shared" si="2"/>
+        <v>34.200000000000003</v>
+      </c>
+      <c r="L5" s="30">
+        <f t="shared" si="3"/>
+        <v>5.32</v>
+      </c>
+      <c r="M5" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I5" s="8">
-        <f t="shared" si="5"/>
-        <v>38.799999999999997</v>
-      </c>
-      <c r="J5" s="8">
-        <f t="shared" si="0"/>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="K5" s="8">
-        <f t="shared" si="1"/>
-        <v>29.7</v>
-      </c>
-      <c r="L5" s="8">
-        <f t="shared" si="2"/>
-        <v>5.3</v>
-      </c>
-      <c r="M5" s="9">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="8">
@@ -862,10 +930,10 @@
         <v>2301</v>
       </c>
       <c r="D6" s="8">
+        <v>2071</v>
+      </c>
+      <c r="E6" s="8">
         <v>2142</v>
-      </c>
-      <c r="E6" s="8">
-        <v>2071</v>
       </c>
       <c r="F6" s="8">
         <v>466</v>
@@ -873,33 +941,33 @@
       <c r="G6" s="9">
         <v>437</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="0"/>
+        <v>20.54</v>
+      </c>
+      <c r="J6" s="30">
+        <f t="shared" si="1"/>
+        <v>18.489999999999998</v>
+      </c>
+      <c r="K6" s="30">
+        <f t="shared" si="2"/>
+        <v>19.13</v>
+      </c>
+      <c r="L6" s="30">
+        <f t="shared" si="3"/>
+        <v>4.16</v>
+      </c>
+      <c r="M6" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <f t="shared" si="5"/>
-        <v>20.5</v>
-      </c>
-      <c r="J6" s="8">
-        <f t="shared" si="0"/>
-        <v>19.100000000000001</v>
-      </c>
-      <c r="K6" s="8">
-        <f t="shared" si="1"/>
-        <v>18.5</v>
-      </c>
-      <c r="L6" s="8">
-        <f t="shared" si="2"/>
-        <v>4.2</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="3"/>
         <v>3.9</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="8">
@@ -909,10 +977,10 @@
         <v>1824</v>
       </c>
       <c r="D7" s="8">
+        <v>1455</v>
+      </c>
+      <c r="E7" s="8">
         <v>2182</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1455</v>
       </c>
       <c r="F7" s="8">
         <v>347</v>
@@ -920,33 +988,33 @@
       <c r="G7" s="9">
         <v>320</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="0"/>
+        <v>27.22</v>
+      </c>
+      <c r="J7" s="30">
+        <f t="shared" si="1"/>
+        <v>21.72</v>
+      </c>
+      <c r="K7" s="30">
+        <f t="shared" si="2"/>
+        <v>32.57</v>
+      </c>
+      <c r="L7" s="30">
+        <f t="shared" si="3"/>
+        <v>5.18</v>
+      </c>
+      <c r="M7" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="5"/>
-        <v>27.2</v>
-      </c>
-      <c r="J7" s="8">
-        <f t="shared" si="0"/>
-        <v>32.6</v>
-      </c>
-      <c r="K7" s="8">
-        <f t="shared" si="1"/>
-        <v>21.7</v>
-      </c>
-      <c r="L7" s="8">
-        <f t="shared" si="2"/>
-        <v>5.2</v>
-      </c>
-      <c r="M7" s="9">
-        <f t="shared" si="3"/>
-        <v>4.8</v>
+        <v>4.78</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="8">
@@ -956,10 +1024,10 @@
         <v>1924</v>
       </c>
       <c r="D8" s="8">
+        <v>1302</v>
+      </c>
+      <c r="E8" s="8">
         <v>1527</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1302</v>
       </c>
       <c r="F8" s="8">
         <v>440</v>
@@ -967,33 +1035,33 @@
       <c r="G8" s="9">
         <v>412</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="0"/>
+        <v>22.9</v>
+      </c>
+      <c r="J8" s="30">
+        <f t="shared" si="1"/>
+        <v>15.5</v>
+      </c>
+      <c r="K8" s="30">
+        <f t="shared" si="2"/>
+        <v>18.18</v>
+      </c>
+      <c r="L8" s="30">
+        <f t="shared" si="3"/>
+        <v>5.24</v>
+      </c>
+      <c r="M8" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="5"/>
-        <v>22.9</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="shared" si="0"/>
-        <v>18.2</v>
-      </c>
-      <c r="K8" s="8">
-        <f t="shared" si="1"/>
-        <v>15.5</v>
-      </c>
-      <c r="L8" s="8">
-        <f t="shared" si="2"/>
-        <v>5.2</v>
-      </c>
-      <c r="M8" s="9">
-        <f t="shared" si="3"/>
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="8">
@@ -1003,10 +1071,10 @@
         <v>2264</v>
       </c>
       <c r="D9" s="8">
+        <v>1432</v>
+      </c>
+      <c r="E9" s="8">
         <v>1455</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1432</v>
       </c>
       <c r="F9" s="8">
         <v>342</v>
@@ -1014,33 +1082,33 @@
       <c r="G9" s="9">
         <v>307</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="0"/>
+        <v>31.01</v>
+      </c>
+      <c r="J9" s="30">
+        <f t="shared" si="1"/>
+        <v>19.62</v>
+      </c>
+      <c r="K9" s="30">
+        <f t="shared" si="2"/>
+        <v>19.93</v>
+      </c>
+      <c r="L9" s="30">
+        <f t="shared" si="3"/>
+        <v>4.68</v>
+      </c>
+      <c r="M9" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" si="5"/>
-        <v>31</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="shared" si="0"/>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" si="1"/>
-        <v>19.600000000000001</v>
-      </c>
-      <c r="L9" s="8">
-        <f t="shared" si="2"/>
-        <v>4.7</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" si="3"/>
-        <v>4.2</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="8">
@@ -1050,10 +1118,10 @@
         <v>4232</v>
       </c>
       <c r="D10" s="8">
+        <v>2298</v>
+      </c>
+      <c r="E10" s="8">
         <v>1743</v>
-      </c>
-      <c r="E10" s="8">
-        <v>2298</v>
       </c>
       <c r="F10" s="8">
         <v>436</v>
@@ -1061,33 +1129,33 @@
       <c r="G10" s="9">
         <v>381</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="0"/>
+        <v>39.92</v>
+      </c>
+      <c r="J10" s="30">
+        <f t="shared" si="1"/>
+        <v>21.68</v>
+      </c>
+      <c r="K10" s="30">
+        <f t="shared" si="2"/>
+        <v>16.440000000000001</v>
+      </c>
+      <c r="L10" s="30">
+        <f t="shared" si="3"/>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="M10" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" si="5"/>
-        <v>39.9</v>
-      </c>
-      <c r="J10" s="8">
-        <f t="shared" si="0"/>
-        <v>16.399999999999999</v>
-      </c>
-      <c r="K10" s="8">
-        <f t="shared" si="1"/>
-        <v>21.7</v>
-      </c>
-      <c r="L10" s="8">
-        <f t="shared" si="2"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="M10" s="9">
-        <f t="shared" si="3"/>
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="8">
@@ -1097,10 +1165,10 @@
         <v>3155</v>
       </c>
       <c r="D11" s="8">
+        <v>3440</v>
+      </c>
+      <c r="E11" s="8">
         <v>1760</v>
-      </c>
-      <c r="E11" s="8">
-        <v>3440</v>
       </c>
       <c r="F11" s="8">
         <v>627</v>
@@ -1108,33 +1176,33 @@
       <c r="G11" s="9">
         <v>575</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="0"/>
+        <v>20.49</v>
+      </c>
+      <c r="J11" s="30">
+        <f t="shared" si="1"/>
+        <v>22.34</v>
+      </c>
+      <c r="K11" s="30">
+        <f t="shared" si="2"/>
+        <v>11.43</v>
+      </c>
+      <c r="L11" s="30">
+        <f t="shared" si="3"/>
+        <v>4.07</v>
+      </c>
+      <c r="M11" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I11" s="8">
-        <f t="shared" si="5"/>
-        <v>20.5</v>
-      </c>
-      <c r="J11" s="8">
-        <f t="shared" si="0"/>
-        <v>11.4</v>
-      </c>
-      <c r="K11" s="8">
-        <f t="shared" si="1"/>
-        <v>22.3</v>
-      </c>
-      <c r="L11" s="8">
-        <f t="shared" si="2"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="3"/>
-        <v>3.7</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="8">
@@ -1144,10 +1212,10 @@
         <v>553</v>
       </c>
       <c r="D12" s="8">
+        <v>131</v>
+      </c>
+      <c r="E12" s="8">
         <v>189</v>
-      </c>
-      <c r="E12" s="8">
-        <v>131</v>
       </c>
       <c r="F12" s="8">
         <v>104</v>
@@ -1155,33 +1223,33 @@
       <c r="G12" s="9">
         <v>103</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="0"/>
+        <v>24.04</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+      <c r="K12" s="30">
+        <f t="shared" si="2"/>
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="L12" s="30">
+        <f t="shared" si="3"/>
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="M12" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="8">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="J12" s="8">
-        <f t="shared" si="0"/>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="K12" s="8">
-        <f t="shared" si="1"/>
-        <v>5.7</v>
-      </c>
-      <c r="L12" s="8">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>4.4800000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8">
@@ -1191,10 +1259,10 @@
         <v>2862</v>
       </c>
       <c r="D13" s="8">
+        <v>2047</v>
+      </c>
+      <c r="E13" s="8">
         <v>1521</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2047</v>
       </c>
       <c r="F13" s="8">
         <v>526</v>
@@ -1202,33 +1270,33 @@
       <c r="G13" s="9">
         <v>479</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="0"/>
+        <v>25.11</v>
+      </c>
+      <c r="J13" s="30">
+        <f t="shared" si="1"/>
+        <v>17.96</v>
+      </c>
+      <c r="K13" s="30">
+        <f t="shared" si="2"/>
+        <v>13.34</v>
+      </c>
+      <c r="L13" s="30">
+        <f t="shared" si="3"/>
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="M13" s="31">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="8">
-        <f t="shared" si="5"/>
-        <v>25.1</v>
-      </c>
-      <c r="J13" s="8">
-        <f t="shared" si="0"/>
-        <v>13.3</v>
-      </c>
-      <c r="K13" s="8">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L13" s="8">
-        <f t="shared" si="2"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="3"/>
         <v>4.2</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="12">
@@ -1238,40 +1306,93 @@
         <v>2363</v>
       </c>
       <c r="D14" s="12">
+        <v>2090</v>
+      </c>
+      <c r="E14" s="12">
         <v>1387</v>
-      </c>
-      <c r="E14" s="12">
-        <v>2090</v>
       </c>
       <c r="F14" s="12">
         <v>457</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="14">
         <v>385</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="16">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="32">
+        <f t="shared" si="0"/>
+        <v>20.2</v>
+      </c>
+      <c r="J14" s="32">
+        <f t="shared" si="1"/>
+        <v>17.86</v>
+      </c>
+      <c r="K14" s="32">
+        <f t="shared" si="2"/>
+        <v>11.85</v>
+      </c>
+      <c r="L14" s="32">
+        <f t="shared" si="3"/>
+        <v>3.91</v>
+      </c>
+      <c r="M14" s="33">
         <f t="shared" si="4"/>
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="25">
+        <f>AVERAGE(B3:B14)</f>
+        <v>86.5</v>
+      </c>
+      <c r="C15" s="28">
+        <f t="shared" ref="C15:M15" si="6">AVERAGE(C3:C14)</f>
+        <v>2317.9166666666665</v>
+      </c>
+      <c r="D15" s="28">
+        <f t="shared" si="6"/>
+        <v>1744.1666666666667</v>
+      </c>
+      <c r="E15" s="28">
+        <f t="shared" ref="E15" si="7">AVERAGE(E3:E14)</f>
+        <v>1570.0833333333333</v>
+      </c>
+      <c r="F15" s="28">
+        <f t="shared" si="6"/>
+        <v>381.5</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="6"/>
+        <v>342.75</v>
+      </c>
+      <c r="H15" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="I14" s="12">
-        <f t="shared" si="5"/>
-        <v>20.2</v>
-      </c>
-      <c r="J14" s="12">
-        <f t="shared" si="0"/>
-        <v>11.9</v>
-      </c>
-      <c r="K14" s="12">
-        <f t="shared" si="1"/>
-        <v>17.899999999999999</v>
-      </c>
-      <c r="L14" s="12">
-        <f t="shared" si="2"/>
-        <v>3.9</v>
-      </c>
-      <c r="M14" s="17">
-        <f t="shared" si="3"/>
-        <v>3.3</v>
+      <c r="I15" s="26">
+        <f t="shared" si="6"/>
+        <v>28.060000000000002</v>
+      </c>
+      <c r="J15" s="26">
+        <f>AVERAGE(J3:J14)</f>
+        <v>19.89916666666667</v>
+      </c>
+      <c r="K15" s="26">
+        <f>AVERAGE(K3:K14)</f>
+        <v>19.852500000000003</v>
+      </c>
+      <c r="L15" s="26">
+        <f t="shared" si="6"/>
+        <v>4.5333333333333323</v>
+      </c>
+      <c r="M15" s="27">
+        <f t="shared" si="6"/>
+        <v>4.0825000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -1281,6 +1402,7 @@
     <mergeCell ref="H1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2171,6 +2293,514 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C762C270-E15B-48EC-88DE-5EC0EE16D709}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.17400002479553</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.2039999961853001</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.2790000438690099</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1.2260000705718901</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1.3309998512268</v>
+      </c>
+      <c r="G2">
+        <f>GEOMEAN(B2:F2)</f>
+        <v>1.241557193752294</v>
+      </c>
+      <c r="H2">
+        <f>ROUND(G2*1000,0)</f>
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2.2379999160766602</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2.1100001335143999</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2.0639998912811199</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2.1399998664855899</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2.0349998474121</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="0">GEOMEAN(B3:F3)</f>
+        <v>2.1162456051168483</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="1">ROUND(G3*1000,0)</f>
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1.29999995231628</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1.29900002479553</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.27200007438659</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.3470001220703101</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1.3150000572204501</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1.3063712312429114</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.84299993515014</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2.0039999485015798</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2.10199999809265</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2.2130000591278001</v>
+      </c>
+      <c r="F5" s="7">
+        <v>2.2200000286102202</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.0714670453714867</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1.4479999542236299</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1.43400001525878</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.4299998283386199</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.50399994850158</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.4579999446868801</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.4545605467329747</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1.21499991416931</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1.2260000705718901</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1.3720002174377399</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.30800008773803</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.39800000190734</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.3016888163233431</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1.4390001296996999</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1.38800001144409</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.43700003623962</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.43299984931945</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1.4659998416900599</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.4323773006918907</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2.22699999809265</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2.2449998855590798</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2.4760000705718901</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2.29900002479553</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.2976386985204065</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3.22699999809265</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3.2969999313354399</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3.2339999675750701</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.63800001144409</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3.8489999771118102</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3.440120884784037</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.12599992752075101</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.13199996948242099</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.13700008392333901</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.13300013542175201</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.12699985504150299</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.13093750268209392</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2.0569999217986998</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2.0139999389648402</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2.06599998474121</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2.0479998588561998</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2.0509998798370299</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.0471229159373361</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1.9630000591278001</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.99500012397766</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2.10199999809265</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2.1509997844696001</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2.0896029234572557</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="3:8">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="3:8">
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9601A82D-B5D6-4F4A-A9E4-CD2835F63018}">
   <dimension ref="A1:H27"/>
   <sheetViews>
@@ -2583,514 +3213,6 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C762C270-E15B-48EC-88DE-5EC0EE16D709}">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1.17400002479553</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1.2039999961853001</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1.2790000438690099</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1.2260000705718901</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1.3309998512268</v>
-      </c>
-      <c r="G2">
-        <f>GEOMEAN(B2:F2)</f>
-        <v>1.241557193752294</v>
-      </c>
-      <c r="H2">
-        <f>ROUND(G2*1000,0)</f>
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2.2379999160766602</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2.1100001335143999</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2.0639998912811199</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2.1399998664855899</v>
-      </c>
-      <c r="F3" s="7">
-        <v>2.0349998474121</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G13" si="0">GEOMEAN(B3:F3)</f>
-        <v>2.1162456051168483</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H13" si="1">ROUND(G3*1000,0)</f>
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1.29999995231628</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1.29900002479553</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1.27200007438659</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1.3470001220703101</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1.3150000572204501</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>1.3063712312429114</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1.84299993515014</v>
-      </c>
-      <c r="C5" s="7">
-        <v>2.0039999485015798</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2.10199999809265</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2.2130000591278001</v>
-      </c>
-      <c r="F5" s="7">
-        <v>2.2200000286102202</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>2.0714670453714867</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>2071</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1.4479999542236299</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1.43400001525878</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1.4299998283386199</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1.50399994850158</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1.4579999446868801</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1.4545605467329747</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1.21499991416931</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1.2260000705718901</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1.3720002174377399</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1.30800008773803</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1.39800000190734</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1.3016888163233431</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1.4390001296996999</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1.38800001144409</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1.43700003623962</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1.43299984931945</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1.4659998416900599</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>1.4323773006918907</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2.22699999809265</v>
-      </c>
-      <c r="C9" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2.2449998855590798</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2.4760000705718901</v>
-      </c>
-      <c r="F9" s="7">
-        <v>2.29900002479553</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>2.2976386985204065</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2298</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7">
-        <v>3.22699999809265</v>
-      </c>
-      <c r="C10" s="7">
-        <v>3.2969999313354399</v>
-      </c>
-      <c r="D10" s="7">
-        <v>3.2339999675750701</v>
-      </c>
-      <c r="E10" s="7">
-        <v>3.63800001144409</v>
-      </c>
-      <c r="F10" s="7">
-        <v>3.8489999771118102</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>3.440120884784037</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>3440</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.12599992752075101</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0.13199996948242099</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.13700008392333901</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.13300013542175201</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0.12699985504150299</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0.13093750268209392</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7">
-        <v>2.0569999217986998</v>
-      </c>
-      <c r="C12" s="7">
-        <v>2.0139999389648402</v>
-      </c>
-      <c r="D12" s="7">
-        <v>2.06599998474121</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2.0479998588561998</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2.0509998798370299</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>2.0471229159373361</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>2047</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1.9630000591278001</v>
-      </c>
-      <c r="C13" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="D13" s="7">
-        <v>1.99500012397766</v>
-      </c>
-      <c r="E13" s="7">
-        <v>2.10199999809265</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2.1509997844696001</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>2.0896029234572557</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="2:8">
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="3:8">
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="3:8">
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="3:8">
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>